<commit_message>
add controls to s1609_gd2car analysis
</commit_message>
<xml_diff>
--- a/template_examples/cytof_s1609_gd2car_analysis_template.xlsx
+++ b/template_examples/cytof_s1609_gd2car_analysis_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441F43E8-8753-CB4D-829D-EBF25EC426CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5072A8BE-F4E6-C943-A6E4-13101389409A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,16 +85,25 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Path to a file on a user's computer.
-In .zip format</t>
+          <t xml:space="preserve">Path to a file on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .zip format</t>
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -121,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -135,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -149,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -163,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -177,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -191,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -210,7 +219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="54">
   <si>
     <t>LEGEND</t>
   </si>
@@ -305,6 +314,12 @@
     <t>#data</t>
   </si>
   <si>
+    <t>Control files package</t>
+  </si>
+  <si>
+    <t>batch1/control_files_analysis.zip</t>
+  </si>
+  <si>
     <t>test_prism_trial_id_run_1</t>
   </si>
   <si>
@@ -372,7 +387,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,6 +406,12 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -486,10 +507,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -828,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2009"/>
+  <dimension ref="A1:I2010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -843,10 +864,10 @@
       <c r="A1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -856,7 +877,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -867,7 +888,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -878,7 +899,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -889,10 +910,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -900,115 +921,121 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" t="s">
-        <v>43</v>
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="I11" t="s">
         <v>45</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>30</v>
       </c>
+      <c r="B12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -10992,13 +11019,18 @@
     </row>
     <row r="2009" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2009" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2010" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2010" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B9:I9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>